<commit_message>
data work and also poster stuff
</commit_message>
<xml_diff>
--- a/FLEX_RUNS.xlsx
+++ b/FLEX_RUNS.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kyroyo\rosetta-antibody-ddgs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59099870-7E6A-4A9D-AC9E-FE4E92C50E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{675007E7-60C3-4388-9068-DE0446C67ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19410" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19410" windowHeight="13875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ddg_run_12_3_r_FLEX" sheetId="1" r:id="rId1"/>
     <sheet name="8 5 r" sheetId="3" r:id="rId2"/>
     <sheet name="8 5 r s" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="stats" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ddg_run_12_3_r_FLEX!$C$1:$C$121</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet1!$A$1:$F$440</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2658" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2661" uniqueCount="404">
   <si>
     <t>#PDB</t>
   </si>
@@ -1248,6 +1250,9 @@
   </si>
   <si>
     <t>8 5 r s</t>
+  </si>
+  <si>
+    <t>MAE</t>
   </si>
 </sst>
 </file>
@@ -17153,15 +17158,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H440"/>
+  <dimension ref="A1:F440"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17180,11 +17185,8 @@
       <c r="F1" t="s">
         <v>402</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -17203,12 +17205,8 @@
       <c r="F2">
         <v>3.1689629082990902</v>
       </c>
-      <c r="H2">
-        <f>PEARSON(C:C, E:E)</f>
-        <v>0.29296842131693884</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -17227,12 +17225,8 @@
       <c r="F3">
         <v>1.7873377340274601</v>
       </c>
-      <c r="H3">
-        <f>PEARSON(C:C, F:F)</f>
-        <v>0.32272158865017125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -17252,7 +17246,7 @@
         <v>4.6234954617491804</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -17272,7 +17266,7 @@
         <v>1.36539448743515</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -17292,7 +17286,7 @@
         <v>5.6037654289007097</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -17312,7 +17306,7 @@
         <v>0.30172093561222901</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -17332,7 +17326,7 @@
         <v>3.72016407877235</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -17352,7 +17346,7 @@
         <v>0.44856315235037902</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -17372,7 +17366,7 @@
         <v>2.2910271269785798</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -17392,7 +17386,7 @@
         <v>-0.104805615613258</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -17412,7 +17406,7 @@
         <v>1.0088723063417999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -17432,7 +17426,7 @@
         <v>2.0299685869166701</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -17452,7 +17446,7 @@
         <v>0.25283989082390601</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -17472,7 +17466,7 @@
         <v>0.84440352794235796</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -24893,6 +24887,48 @@
       </c>
       <c r="D440" t="s">
         <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F440" xr:uid="{00000000-0001-0000-0300-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283CCA3F-6521-487A-843F-907DCE41724E}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B2">
+        <f>PEARSON(Sheet1!C:C, Sheet1!E:E)</f>
+        <v>0.29296842131693884</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B3">
+        <f>PEARSON(Sheet1!C:C, Sheet1!F:F)</f>
+        <v>0.32272158865017125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FLEX_RUNS changes and minimal runs beginning
</commit_message>
<xml_diff>
--- a/FLEX_RUNS.xlsx
+++ b/FLEX_RUNS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\kyroyo\rosetta-antibody-ddgs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310FB8C4-0AB0-49D5-90C0-243F4A17BE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F98E5F-A92D-4F48-8916-7E9A17507379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19410" windowHeight="13875" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19410" windowHeight="13875" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ddg_run_12_3_r_FLEX" sheetId="1" r:id="rId1"/>
@@ -8220,18 +8220,36 @@
                 <c:pt idx="1">
                   <c:v>1.93515062459818</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8545177084597801</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4571616846454001</c:v>
+                </c:pt>
                 <c:pt idx="10">
                   <c:v>1.06102511235792</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.92241468420712402</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.114993611286327</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.9925532014449299E-2</c:v>
+                </c:pt>
                 <c:pt idx="60">
                   <c:v>-0.255010662886206</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>-1.9675810496485699</c:v>
                 </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.1224662313634301E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.61429707729462202</c:v>
+                </c:pt>
                 <c:pt idx="91">
                   <c:v>4.5844647546288799</c:v>
                 </c:pt>
@@ -8239,10 +8257,16 @@
                   <c:v>2.0979674336762799</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.76917968846523299</c:v>
+                  <c:v>-0.16315301425116499</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>-7.6001913827421899E-2</c:v>
+                  <c:v>-0.17209986442245201</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.6532270115464902</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-7.1521434147052698E-2</c:v>
                 </c:pt>
                 <c:pt idx="131">
                   <c:v>7.0996986661102698E-2</c:v>
@@ -8250,12 +8274,24 @@
                 <c:pt idx="132">
                   <c:v>0.17140020238072701</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>-0.42552363206645999</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.57318300111273E-2</c:v>
+                </c:pt>
                 <c:pt idx="230">
                   <c:v>2.2259462434990902</c:v>
                 </c:pt>
                 <c:pt idx="231">
                   <c:v>-0.20335409103658</c:v>
                 </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.7546391371547401</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.43154289143096303</c:v>
+                </c:pt>
                 <c:pt idx="251">
                   <c:v>-4.7634741345402203</c:v>
                 </c:pt>
@@ -8271,6 +8307,12 @@
                 <c:pt idx="259">
                   <c:v>4.0089537872576697</c:v>
                 </c:pt>
+                <c:pt idx="260">
+                  <c:v>1.18241154441592</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>-2.1118085350508398E-2</c:v>
+                </c:pt>
                 <c:pt idx="285">
                   <c:v>6.5892851582102493E-2</c:v>
                 </c:pt>
@@ -8283,30 +8325,60 @@
                 <c:pt idx="288">
                   <c:v>6.3860986058307896</c:v>
                 </c:pt>
+                <c:pt idx="289">
+                  <c:v>4.3572243571501899</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>5.25249875392542</c:v>
+                </c:pt>
                 <c:pt idx="291">
                   <c:v>-0.43985307182051597</c:v>
                 </c:pt>
                 <c:pt idx="292">
                   <c:v>-4.1210328193525703</c:v>
                 </c:pt>
+                <c:pt idx="293">
+                  <c:v>-2.6925482187320302</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>-1.6095053532035399</c:v>
+                </c:pt>
                 <c:pt idx="295">
                   <c:v>-3.7438834323291701</c:v>
                 </c:pt>
                 <c:pt idx="296">
                   <c:v>0.18982700571496</c:v>
                 </c:pt>
+                <c:pt idx="297">
+                  <c:v>0.27235917544872701</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>2.7022852747133501</c:v>
+                </c:pt>
                 <c:pt idx="299">
                   <c:v>-3.5652570672162298</c:v>
                 </c:pt>
                 <c:pt idx="300">
                   <c:v>-1.35137464813269</c:v>
                 </c:pt>
+                <c:pt idx="301">
+                  <c:v>0.66969967021285803</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>1.51651330546628</c:v>
+                </c:pt>
                 <c:pt idx="303">
                   <c:v>-0.27194963070406603</c:v>
                 </c:pt>
                 <c:pt idx="304">
                   <c:v>1.97288343595895</c:v>
                 </c:pt>
+                <c:pt idx="305">
+                  <c:v>3.9728991813169099</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>5.4558430672037304</c:v>
+                </c:pt>
                 <c:pt idx="317">
                   <c:v>-0.53914752540131305</c:v>
                 </c:pt>
@@ -8316,18 +8388,36 @@
                 <c:pt idx="319">
                   <c:v>4.7698990042701404</c:v>
                 </c:pt>
+                <c:pt idx="320">
+                  <c:v>0.294959002964296</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>2.9544510025566399</c:v>
+                </c:pt>
                 <c:pt idx="328">
                   <c:v>9.2451568851447501E-3</c:v>
                 </c:pt>
                 <c:pt idx="329">
                   <c:v>-0.926101205304657</c:v>
                 </c:pt>
+                <c:pt idx="330">
+                  <c:v>0.52803081818935405</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>9.5748779825989894E-2</c:v>
+                </c:pt>
                 <c:pt idx="333">
                   <c:v>-2.7200947622460299</c:v>
                 </c:pt>
                 <c:pt idx="334">
                   <c:v>-4.31615855779076</c:v>
                 </c:pt>
+                <c:pt idx="335">
+                  <c:v>-2.0502628354242901E-2</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>-2.6766325079352098E-2</c:v>
+                </c:pt>
                 <c:pt idx="381">
                   <c:v>-0.119417880560895</c:v>
                 </c:pt>
@@ -8335,10 +8425,16 @@
                   <c:v>0.97745942203976199</c:v>
                 </c:pt>
                 <c:pt idx="383">
-                  <c:v>-0.39729046514652899</c:v>
+                  <c:v>-0.227861375864335</c:v>
                 </c:pt>
                 <c:pt idx="384">
-                  <c:v>1.49201197353681</c:v>
+                  <c:v>1.7420039192239001</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>0.25220496826012301</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>2.6757311355870299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18407,7 +18503,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{E9E3F1BD-F665-4720-8DBA-8608855B5472}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -27901,15 +27997,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M440"/>
+  <dimension ref="A1:O440"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -27946,11 +28042,11 @@
       <c r="L1" t="s">
         <v>410</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -27987,12 +28083,12 @@
       <c r="L2">
         <v>3.5026393269999998</v>
       </c>
-      <c r="M2">
-        <f>ABS(L2-C2)</f>
-        <v>1.5026393269999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O2">
+        <f>ABS(H2-C2)</f>
+        <v>1.3494970193031599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -28029,12 +28125,12 @@
       <c r="L3">
         <v>2.0452196819999999</v>
       </c>
-      <c r="M3">
-        <f>ABS(L3-C3)</f>
-        <v>2.8547803180000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O3">
+        <f t="shared" ref="O3:O66" si="0">ABS(H3-C3)</f>
+        <v>2.9648493754018204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -28056,6 +28152,9 @@
       <c r="G4">
         <v>4.9362524519054203</v>
       </c>
+      <c r="H4">
+        <v>4.8545177084597801</v>
+      </c>
       <c r="I4">
         <v>5.0543032602527997</v>
       </c>
@@ -28065,8 +28164,12 @@
       <c r="K4">
         <v>5.6196484734869001</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.64548229154021985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -28088,6 +28191,9 @@
       <c r="G5">
         <v>2.2274743302853399</v>
       </c>
+      <c r="H5">
+        <v>2.4571616846454001</v>
+      </c>
       <c r="I5">
         <v>2.5477269126756199</v>
       </c>
@@ -28097,8 +28203,12 @@
       <c r="K5">
         <v>0.88799075139404504</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>4.4428383153546003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -28130,7 +28240,7 @@
         <v>5.0267024274175096</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -28162,7 +28272,7 @@
         <v>0.27175650932604101</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -28194,7 +28304,7 @@
         <v>2.7914631778896299</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -28226,7 +28336,7 @@
         <v>0.59161791763863203</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -28258,7 +28368,7 @@
         <v>1.5727244988782301</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -28290,7 +28400,7 @@
         <v>-0.47505551725289402</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -28327,12 +28437,12 @@
       <c r="L12">
         <v>1.59491204555397</v>
       </c>
-      <c r="M12">
-        <f t="shared" ref="M4:M67" si="0">ABS(L12-C12)</f>
-        <v>1.59491204555397</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>1.06102511235792</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -28369,12 +28479,12 @@
       <c r="L13">
         <v>1.5755805880939899</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <f t="shared" si="0"/>
-        <v>0.81558058809398992</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.16241468420712402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -28396,6 +28506,9 @@
       <c r="G14">
         <v>0.47285547315332199</v>
       </c>
+      <c r="H14">
+        <v>0.114993611286327</v>
+      </c>
       <c r="I14">
         <v>0.63660270133541397</v>
       </c>
@@ -28405,8 +28518,12 @@
       <c r="K14">
         <v>0.20955974914922901</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O14">
+        <f t="shared" si="0"/>
+        <v>0.45500638871367294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -28428,6 +28545,9 @@
       <c r="G15">
         <v>-0.120895213155699</v>
       </c>
+      <c r="H15">
+        <v>-1.9925532014449299E-2</v>
+      </c>
       <c r="I15">
         <v>-0.16674214833401399</v>
       </c>
@@ -28437,8 +28557,12 @@
       <c r="K15">
         <v>4.8412643079245699E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>2.7499255320144491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -29092,7 +29216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -29106,7 +29230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -29120,7 +29244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -29134,7 +29258,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -29148,7 +29272,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -29162,7 +29286,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -29176,7 +29300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -29190,7 +29314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -29204,7 +29328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -29218,7 +29342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -29232,7 +29356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -29246,7 +29370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -29260,7 +29384,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -29274,7 +29398,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -29308,12 +29432,12 @@
       <c r="L62">
         <v>-0.98575262745976</v>
       </c>
-      <c r="M62">
+      <c r="O62">
         <f t="shared" si="0"/>
-        <v>0.60575262745976</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.12498933711379401</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -29347,12 +29471,12 @@
       <c r="L63">
         <v>-1.0060018294388999</v>
       </c>
-      <c r="M63">
+      <c r="O63">
         <f t="shared" si="0"/>
-        <v>0.51600182943889994</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.47758104964857</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -29374,14 +29498,21 @@
       <c r="G64">
         <v>0.327797071859458</v>
       </c>
+      <c r="H64">
+        <v>1.1224662313634301E-2</v>
+      </c>
       <c r="I64">
         <v>-0.163064651707372</v>
       </c>
       <c r="J64">
         <v>-2.4935719854370202</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O64">
+        <f t="shared" si="0"/>
+        <v>0.1612246623136343</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -29403,14 +29534,21 @@
       <c r="G65">
         <v>-0.37486974367384301</v>
       </c>
+      <c r="H65">
+        <v>0.61429707729462202</v>
+      </c>
       <c r="I65">
         <v>0.61262348751324602</v>
       </c>
       <c r="J65">
         <v>0.466763357530453</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O65">
+        <f t="shared" si="0"/>
+        <v>0.16429707729462201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -29439,7 +29577,7 @@
         <v>-0.211377502591858</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -29468,7 +29606,7 @@
         <v>-3.26840576922713</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -29497,7 +29635,7 @@
         <v>-1.28948135152486</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -29526,7 +29664,7 @@
         <v>0.69647794081138203</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -29552,7 +29690,7 @@
         <v>-1.50158861074341</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -29578,7 +29716,7 @@
         <v>-0.34358904776318</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>5</v>
       </c>
@@ -29603,12 +29741,8 @@
       <c r="L72">
         <v>0.20487142332785799</v>
       </c>
-      <c r="M72">
-        <f t="shared" ref="M68:M131" si="1">ABS(L72-C72)</f>
-        <v>4.5128576672142012E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>5</v>
       </c>
@@ -29633,12 +29767,8 @@
       <c r="L73">
         <v>5.2458900197780101E-2</v>
       </c>
-      <c r="M73">
-        <f t="shared" si="1"/>
-        <v>0.55754109980221989</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>5</v>
       </c>
@@ -29661,7 +29791,7 @@
         <v>-0.121904193962291</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>5</v>
       </c>
@@ -29684,7 +29814,7 @@
         <v>3.3184795746537898</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>5</v>
       </c>
@@ -29701,7 +29831,7 @@
         <v>0.108804922980016</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>5</v>
       </c>
@@ -29718,7 +29848,7 @@
         <v>-0.456172575713571</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>5</v>
       </c>
@@ -29735,7 +29865,7 @@
         <v>3.42455165453757</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>5</v>
       </c>
@@ -29752,7 +29882,7 @@
         <v>-8.4547785001086506E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>5</v>
       </c>
@@ -29766,7 +29896,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>5</v>
       </c>
@@ -29780,7 +29910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -29794,7 +29924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>5</v>
       </c>
@@ -29808,7 +29938,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>5</v>
       </c>
@@ -29822,7 +29952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>5</v>
       </c>
@@ -29836,7 +29966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -29850,7 +29980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>5</v>
       </c>
@@ -29864,7 +29994,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>5</v>
       </c>
@@ -29878,7 +30008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>5</v>
       </c>
@@ -29892,7 +30022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>5</v>
       </c>
@@ -29906,7 +30036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>5</v>
       </c>
@@ -29920,7 +30050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>5</v>
       </c>
@@ -29934,7 +30064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -29971,12 +30101,12 @@
       <c r="L93">
         <v>5.4822437927943604</v>
       </c>
-      <c r="M93">
-        <f t="shared" si="1"/>
-        <v>2.5822437927943604</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O93">
+        <f t="shared" ref="O67:O130" si="1">ABS(H93-C93)</f>
+        <v>1.68446475462888</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -30013,12 +30143,12 @@
       <c r="L94">
         <v>1.6850264818051699</v>
       </c>
-      <c r="M94">
+      <c r="O94">
         <f t="shared" si="1"/>
-        <v>0.6850264818051699</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.0979674336762799</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -30041,7 +30171,7 @@
         <v>-0.90235981678345001</v>
       </c>
       <c r="H95">
-        <v>0.76917968846523299</v>
+        <v>-0.16315301425116499</v>
       </c>
       <c r="I95">
         <v>-1.7612767212682601</v>
@@ -30052,8 +30182,12 @@
       <c r="K95">
         <v>-0.13120638749678601</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O95">
+        <f t="shared" si="1"/>
+        <v>0.24315301425116498</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -30076,7 +30210,7 @@
         <v>-0.51375960697830503</v>
       </c>
       <c r="H96">
-        <v>-7.6001913827421899E-2</v>
+        <v>-0.17209986442245201</v>
       </c>
       <c r="I96">
         <v>0.41882417827559898</v>
@@ -30087,8 +30221,12 @@
       <c r="K96">
         <v>-8.2088604681894106E-2</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O96">
+        <f t="shared" si="1"/>
+        <v>4.2099864422452005E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -30110,6 +30248,9 @@
       <c r="G97">
         <v>4.0711400011592298</v>
       </c>
+      <c r="H97">
+        <v>3.6532270115464902</v>
+      </c>
       <c r="I97">
         <v>1.18705775333</v>
       </c>
@@ -30119,8 +30260,12 @@
       <c r="K97">
         <v>0.70697203420099797</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O97">
+        <f t="shared" si="1"/>
+        <v>3.3532270115464904</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -30142,6 +30287,9 @@
       <c r="G98">
         <v>-0.90345768157180795</v>
       </c>
+      <c r="H98">
+        <v>-7.1521434147052698E-2</v>
+      </c>
       <c r="I98">
         <v>0.18883544117484199</v>
       </c>
@@ -30151,8 +30299,12 @@
       <c r="K98">
         <v>3.0239911882007098</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O98">
+        <f t="shared" si="1"/>
+        <v>0.43847856585294731</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -30184,7 +30336,7 @@
         <v>0.25847084741130799</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -30216,7 +30368,7 @@
         <v>0.174669352189494</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -30245,7 +30397,7 @@
         <v>-1.9739922587230401</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -30274,7 +30426,7 @@
         <v>-0.11669960819467599</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -30303,7 +30455,7 @@
         <v>0.35873701050040802</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -30332,7 +30484,7 @@
         <v>0.443269906404475</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -30361,7 +30513,7 @@
         <v>-1.2081545412616801</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -30390,7 +30542,7 @@
         <v>5.1863451081713698</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -30419,7 +30571,7 @@
         <v>-4.2052154878277603</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -30448,7 +30600,7 @@
         <v>1.36182971772759</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -30474,7 +30626,7 @@
         <v>0.66971645981639005</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -30500,7 +30652,7 @@
         <v>0.48930706390242401</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -30526,7 +30678,7 @@
         <v>-1.34543789154563</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -30552,7 +30704,7 @@
         <v>-0.31157524412619703</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -30578,7 +30730,7 @@
         <v>-0.35916263898447998</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -30604,7 +30756,7 @@
         <v>4.0376578036378703</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -30630,7 +30782,7 @@
         <v>1.2617647820748901</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>6</v>
       </c>
@@ -30656,7 +30808,7 @@
         <v>-0.54340023114395897</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -30679,7 +30831,7 @@
         <v>1.42213697652368</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>6</v>
       </c>
@@ -30702,7 +30854,7 @@
         <v>-2.23936525058493</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>136</v>
       </c>
@@ -30736,12 +30888,8 @@
       <c r="L119">
         <v>-2.2647896753071102</v>
       </c>
-      <c r="M119">
-        <f t="shared" si="1"/>
-        <v>2.2047896753071101</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>136</v>
       </c>
@@ -30775,12 +30923,8 @@
       <c r="L120">
         <v>-0.34805600700355999</v>
       </c>
-      <c r="M120">
-        <f t="shared" si="1"/>
-        <v>0.28805600700355999</v>
-      </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -30812,7 +30956,7 @@
         <v>0.57523932984822701</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -30844,7 +30988,7 @@
         <v>-4.0568126341895498E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>136</v>
       </c>
@@ -30870,7 +31014,7 @@
         <v>-5.9662362178278201E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>142</v>
       </c>
@@ -30890,7 +31034,7 @@
         <v>3.9626816368217903E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -30910,7 +31054,7 @@
         <v>-0.55926459777692705</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>142</v>
       </c>
@@ -30927,7 +31071,7 @@
         <v>1.7469813585032099</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>142</v>
       </c>
@@ -30944,7 +31088,7 @@
         <v>0.58561232910069505</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -30961,7 +31105,7 @@
         <v>0.67850902319842099</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>142</v>
       </c>
@@ -30978,7 +31122,7 @@
         <v>2.8720344670320599</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>142</v>
       </c>
@@ -30995,7 +31139,7 @@
         <v>2.3659610219725402</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>142</v>
       </c>
@@ -31012,7 +31156,7 @@
         <v>-0.46512684046001501</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>142</v>
       </c>
@@ -31029,7 +31173,7 @@
         <v>2.9692449118448101</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -31066,12 +31210,12 @@
       <c r="L133">
         <v>0.115690236337604</v>
       </c>
-      <c r="M133">
-        <f t="shared" ref="M132:M195" si="2">ABS(L133-C133)</f>
-        <v>8.4309763662396009E-2</v>
-      </c>
-    </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O133">
+        <f t="shared" ref="O131:O194" si="2">ABS(H133-C133)</f>
+        <v>0.1290030133388973</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>151</v>
       </c>
@@ -31108,12 +31252,12 @@
       <c r="L134">
         <v>0.12397392157567901</v>
       </c>
-      <c r="M134">
+      <c r="O134">
         <f t="shared" si="2"/>
-        <v>0.12397392157567901</v>
-      </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.17140020238072701</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -31135,6 +31279,9 @@
       <c r="G135">
         <v>-0.51633205695725304</v>
       </c>
+      <c r="H135">
+        <v>-0.42552363206645999</v>
+      </c>
       <c r="I135">
         <v>-0.31006018750586001</v>
       </c>
@@ -31144,8 +31291,12 @@
       <c r="K135">
         <v>-0.11191415331113599</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O135">
+        <f t="shared" si="2"/>
+        <v>1.1255236320664599</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -31167,6 +31318,9 @@
       <c r="G136">
         <v>-9.73172967948812E-2</v>
       </c>
+      <c r="H136">
+        <v>3.57318300111273E-2</v>
+      </c>
       <c r="I136">
         <v>3.47645384214047E-2</v>
       </c>
@@ -31176,8 +31330,12 @@
       <c r="K136">
         <v>-8.4529548638147295E-2</v>
       </c>
-    </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O136">
+        <f t="shared" si="2"/>
+        <v>0.16426816998887273</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -31209,7 +31367,7 @@
         <v>1.54107985301925</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -31241,7 +31399,7 @@
         <v>0.70053772257106095</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -31273,7 +31431,7 @@
         <v>-6.4574785580498395E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -31305,7 +31463,7 @@
         <v>7.6267535896749894E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>151</v>
       </c>
@@ -31337,7 +31495,7 @@
         <v>0.101482917344856</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>151</v>
       </c>
@@ -31369,7 +31527,7 @@
         <v>0.159834536943435</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>151</v>
       </c>
@@ -31398,7 +31556,7 @@
         <v>8.3416066116114906E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -31747,7 +31905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>151</v>
       </c>
@@ -31761,7 +31919,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>151</v>
       </c>
@@ -31775,7 +31933,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>151</v>
       </c>
@@ -31789,7 +31947,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>151</v>
       </c>
@@ -31803,7 +31961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>151</v>
       </c>
@@ -31817,7 +31975,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>175</v>
       </c>
@@ -31842,12 +32000,8 @@
       <c r="L166">
         <v>-0.203797737998411</v>
       </c>
-      <c r="M166">
-        <f t="shared" si="2"/>
-        <v>0.60379773799841097</v>
-      </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>175</v>
       </c>
@@ -31872,12 +32026,8 @@
       <c r="L167">
         <v>0.15049413421111199</v>
       </c>
-      <c r="M167">
-        <f t="shared" si="2"/>
-        <v>0.250494134211112</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>175</v>
       </c>
@@ -31900,7 +32050,7 @@
         <v>5.7336836377999099E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>175</v>
       </c>
@@ -31923,7 +32073,7 @@
         <v>0.214083417678193</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>175</v>
       </c>
@@ -31940,7 +32090,7 @@
         <v>-1.0884111884714001</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>175</v>
       </c>
@@ -31957,7 +32107,7 @@
         <v>0.39975301578087902</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>175</v>
       </c>
@@ -31974,7 +32124,7 @@
         <v>-0.288780036565913</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>175</v>
       </c>
@@ -31991,7 +32141,7 @@
         <v>-8.7624494631836497E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>175</v>
       </c>
@@ -32008,7 +32158,7 @@
         <v>1.52604135595483</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>175</v>
       </c>
@@ -32025,7 +32175,7 @@
         <v>1.0084427397328</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -32263,7 +32413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>175</v>
       </c>
@@ -32277,7 +32427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>175</v>
       </c>
@@ -32291,7 +32441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>175</v>
       </c>
@@ -32305,7 +32455,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>175</v>
       </c>
@@ -32319,7 +32469,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>175</v>
       </c>
@@ -32333,7 +32483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>175</v>
       </c>
@@ -32347,7 +32497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>175</v>
       </c>
@@ -32361,7 +32511,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>177</v>
       </c>
@@ -32395,12 +32545,8 @@
       <c r="L200">
         <v>3.71096961158998</v>
       </c>
-      <c r="M200">
-        <f t="shared" ref="M196:M257" si="3">ABS(L200-C200)</f>
-        <v>2.3509696115899796</v>
-      </c>
-    </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>177</v>
       </c>
@@ -32434,12 +32580,8 @@
       <c r="L201">
         <v>2.9217909767979702</v>
       </c>
-      <c r="M201">
-        <f t="shared" si="3"/>
-        <v>1.5617909767979701</v>
-      </c>
-    </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>177</v>
       </c>
@@ -32471,7 +32613,7 @@
         <v>4.3728364358566898</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>177</v>
       </c>
@@ -32503,7 +32645,7 @@
         <v>1.53946156795509</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>177</v>
       </c>
@@ -32535,7 +32677,7 @@
         <v>0.164230999981646</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>177</v>
       </c>
@@ -32567,7 +32709,7 @@
         <v>-1.1788819675553801</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>177</v>
       </c>
@@ -32599,7 +32741,7 @@
         <v>4.9159713506950498</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>185</v>
       </c>
@@ -32633,12 +32775,8 @@
       <c r="L207">
         <v>-9.5322119012735101E-2</v>
       </c>
-      <c r="M207">
-        <f t="shared" si="3"/>
-        <v>1.995322119012735</v>
-      </c>
-    </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>185</v>
       </c>
@@ -32672,12 +32810,8 @@
       <c r="L208">
         <v>1.30048956654286</v>
       </c>
-      <c r="M208">
-        <f t="shared" si="3"/>
-        <v>1.13048956654286</v>
-      </c>
-    </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>185</v>
       </c>
@@ -32709,7 +32843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>185</v>
       </c>
@@ -32741,7 +32875,7 @@
         <v>5.6686588614753797</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>185</v>
       </c>
@@ -32773,7 +32907,7 @@
         <v>0.122098307216583</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>185</v>
       </c>
@@ -32805,7 +32939,7 @@
         <v>2.5304977790587602</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>185</v>
       </c>
@@ -32837,7 +32971,7 @@
         <v>2.7269244506094301</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>185</v>
       </c>
@@ -32869,7 +33003,7 @@
         <v>4.0625790849609897</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>185</v>
       </c>
@@ -32901,7 +33035,7 @@
         <v>2.2953300665752501</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>185</v>
       </c>
@@ -32930,7 +33064,7 @@
         <v>-2.0554672321350099E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>185</v>
       </c>
@@ -32956,7 +33090,7 @@
         <v>-0.52109748507368703</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>185</v>
       </c>
@@ -32982,7 +33116,7 @@
         <v>2.7267895797233899</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>185</v>
       </c>
@@ -33008,7 +33142,7 @@
         <v>3.1277811787958798E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>185</v>
       </c>
@@ -33034,7 +33168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>194</v>
       </c>
@@ -33065,12 +33199,8 @@
       <c r="L221">
         <v>2.6372801354144402</v>
       </c>
-      <c r="M221">
-        <f t="shared" si="3"/>
-        <v>2.6972801354144402</v>
-      </c>
-    </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>194</v>
       </c>
@@ -33101,12 +33231,8 @@
       <c r="L222">
         <v>0.93415144859541199</v>
       </c>
-      <c r="M222">
-        <f t="shared" si="3"/>
-        <v>0.20415144859541201</v>
-      </c>
-    </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>194</v>
       </c>
@@ -33135,7 +33261,7 @@
         <v>0.78576197464408304</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>194</v>
       </c>
@@ -33164,7 +33290,7 @@
         <v>0.17806903025548301</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>194</v>
       </c>
@@ -33184,7 +33310,7 @@
         <v>-0.68028751200945403</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>194</v>
       </c>
@@ -33204,7 +33330,7 @@
         <v>5.5571600716848399E-2</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>194</v>
       </c>
@@ -33224,7 +33350,7 @@
         <v>-0.77441736980763298</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>194</v>
       </c>
@@ -33244,7 +33370,7 @@
         <v>-1.4822114758540901</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>194</v>
       </c>
@@ -33264,7 +33390,7 @@
         <v>0.43821369167353602</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>194</v>
       </c>
@@ -33284,7 +33410,7 @@
         <v>-7.8171463264879997E-4</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>194</v>
       </c>
@@ -33301,7 +33427,7 @@
         <v>2.8988753161857801</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>206</v>
       </c>
@@ -33338,12 +33464,12 @@
       <c r="L232">
         <v>1.9342531020520199</v>
       </c>
-      <c r="M232">
-        <f t="shared" si="3"/>
-        <v>0.26425310205202002</v>
-      </c>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O232">
+        <f t="shared" ref="O195:O258" si="3">ABS(H232-C232)</f>
+        <v>0.55594624349909028</v>
+      </c>
+    </row>
+    <row r="233" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>206</v>
       </c>
@@ -33380,12 +33506,12 @@
       <c r="L233">
         <v>0.25907180642448102</v>
       </c>
-      <c r="M233">
+      <c r="O233">
         <f t="shared" si="3"/>
-        <v>0.91092819357551891</v>
-      </c>
-    </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.37335409103658</v>
+      </c>
+    </row>
+    <row r="234" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>206</v>
       </c>
@@ -33407,6 +33533,9 @@
       <c r="G234">
         <v>1.57701870894593</v>
       </c>
+      <c r="H234">
+        <v>1.7546391371547401</v>
+      </c>
       <c r="I234">
         <v>0.62370781031922795</v>
       </c>
@@ -33416,8 +33545,12 @@
       <c r="K234">
         <v>3.1412066710325601</v>
       </c>
-    </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O234">
+        <f t="shared" si="3"/>
+        <v>1.41463913715474</v>
+      </c>
+    </row>
+    <row r="235" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>206</v>
       </c>
@@ -33439,6 +33572,9 @@
       <c r="G235">
         <v>0.75176709387783303</v>
       </c>
+      <c r="H235">
+        <v>0.43154289143096303</v>
+      </c>
       <c r="I235">
         <v>1.33974291987742</v>
       </c>
@@ -33448,8 +33584,12 @@
       <c r="K235">
         <v>0.69667157489598097</v>
       </c>
-    </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O235">
+        <f t="shared" si="3"/>
+        <v>1.6184571085690367</v>
+      </c>
+    </row>
+    <row r="236" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>206</v>
       </c>
@@ -33481,7 +33621,7 @@
         <v>1.6759706232470299</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>206</v>
       </c>
@@ -33513,7 +33653,7 @@
         <v>1.67438943268603</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>206</v>
       </c>
@@ -33542,7 +33682,7 @@
         <v>5.8411310004392298</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>206</v>
       </c>
@@ -33571,7 +33711,7 @@
         <v>14.872242699525801</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>206</v>
       </c>
@@ -33600,7 +33740,7 @@
         <v>4.8039468150403</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>206</v>
       </c>
@@ -33629,7 +33769,7 @@
         <v>3.1300887910902002</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>206</v>
       </c>
@@ -33658,7 +33798,7 @@
         <v>1.4051942844413501</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>206</v>
       </c>
@@ -33687,7 +33827,7 @@
         <v>-0.279994278475169</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>206</v>
       </c>
@@ -33710,7 +33850,7 @@
         <v>0.88529164714518604</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>206</v>
       </c>
@@ -33733,7 +33873,7 @@
         <v>-1.1682706412368999</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>206</v>
       </c>
@@ -33756,7 +33896,7 @@
         <v>2.54490421000264</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>206</v>
       </c>
@@ -33779,7 +33919,7 @@
         <v>-0.53822116654600904</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>206</v>
       </c>
@@ -33802,7 +33942,7 @@
         <v>-0.34489968489287998</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>206</v>
       </c>
@@ -33825,7 +33965,7 @@
         <v>2.4058402423255698</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>206</v>
       </c>
@@ -33848,7 +33988,7 @@
         <v>-6.1318979910678504</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>206</v>
       </c>
@@ -33871,7 +34011,7 @@
         <v>-3.1477255785823202</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>206</v>
       </c>
@@ -33894,7 +34034,7 @@
         <v>-0.87926386998988104</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>227</v>
       </c>
@@ -33931,12 +34071,12 @@
       <c r="L253">
         <v>-4.2108551040854296</v>
       </c>
-      <c r="M253">
+      <c r="O253">
         <f t="shared" si="3"/>
-        <v>1.6154278130854296</v>
-      </c>
-    </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.45">
+        <v>2.1680468435402203</v>
+      </c>
+    </row>
+    <row r="254" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>230</v>
       </c>
@@ -33973,12 +34113,12 @@
       <c r="L254">
         <v>-2.0856736818986001</v>
       </c>
-      <c r="M254">
+      <c r="O254">
         <f t="shared" si="3"/>
-        <v>1.2528417778986003</v>
-      </c>
-    </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.2267215259605302</v>
+      </c>
+    </row>
+    <row r="255" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>232</v>
       </c>
@@ -34015,12 +34155,12 @@
       <c r="L255">
         <v>-2.8095750831634798</v>
       </c>
-      <c r="M255">
+      <c r="O255">
         <f t="shared" si="3"/>
-        <v>1.3666245771634797</v>
-      </c>
-    </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.4468166288881099</v>
+      </c>
+    </row>
+    <row r="256" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>234</v>
       </c>
@@ -34054,12 +34194,8 @@
       <c r="L256">
         <v>2.1287641299791802</v>
       </c>
-      <c r="M256">
-        <f t="shared" si="3"/>
-        <v>2.1287641299791802</v>
-      </c>
-    </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="257" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>234</v>
       </c>
@@ -34093,12 +34229,8 @@
       <c r="L257">
         <v>-3.31882212999502</v>
       </c>
-      <c r="M257">
-        <f t="shared" si="3"/>
-        <v>3.7458238889950199</v>
-      </c>
-    </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="258" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>234</v>
       </c>
@@ -34130,7 +34262,7 @@
         <v>16.5089505899522</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>234</v>
       </c>
@@ -34162,7 +34294,7 @@
         <v>6.7825329799664296</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>239</v>
       </c>
@@ -34199,12 +34331,12 @@
       <c r="L260">
         <v>4.4389026944945398</v>
       </c>
-      <c r="M260">
-        <f t="shared" ref="M260:M321" si="4">ABS(L260-C260)</f>
-        <v>3.8744370724945396</v>
-      </c>
-    </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O260">
+        <f t="shared" ref="O259:O322" si="4">ABS(H260-C260)</f>
+        <v>3.4541829280316696</v>
+      </c>
+    </row>
+    <row r="261" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>239</v>
       </c>
@@ -34241,12 +34373,12 @@
       <c r="L261">
         <v>3.8385921182270502</v>
       </c>
-      <c r="M261">
+      <c r="O261">
         <f t="shared" si="4"/>
-        <v>3.3864426502270502</v>
-      </c>
-    </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.45">
+        <v>3.5568043192576697</v>
+      </c>
+    </row>
+    <row r="262" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>239</v>
       </c>
@@ -34268,14 +34400,21 @@
       <c r="G262">
         <v>1.6193688674073601</v>
       </c>
+      <c r="H262">
+        <v>1.18241154441592</v>
+      </c>
       <c r="J262">
         <v>1.4146209955932101</v>
       </c>
       <c r="K262">
         <v>1.22611653632579</v>
       </c>
-    </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O262">
+        <f t="shared" si="4"/>
+        <v>2.9319034415919987E-2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>239</v>
       </c>
@@ -34297,14 +34436,21 @@
       <c r="G263">
         <v>0.37751416734920401</v>
       </c>
+      <c r="H263">
+        <v>-2.1118085350508398E-2</v>
+      </c>
       <c r="J263">
         <v>0.28734445397262698</v>
       </c>
       <c r="K263">
         <v>2.3437704070920499E-2</v>
       </c>
-    </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O263">
+        <f t="shared" si="4"/>
+        <v>0.6253415863505084</v>
+      </c>
+    </row>
+    <row r="264" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>239</v>
       </c>
@@ -34333,7 +34479,7 @@
         <v>2.6271150994880998</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>239</v>
       </c>
@@ -34362,7 +34508,7 @@
         <v>-0.25467546215286302</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>239</v>
       </c>
@@ -34391,7 +34537,7 @@
         <v>3.1295203688483499</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>239</v>
       </c>
@@ -34420,7 +34566,7 @@
         <v>0.15298583716250899</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>239</v>
       </c>
@@ -34446,7 +34592,7 @@
         <v>2.6958982013481498</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>239</v>
       </c>
@@ -34472,7 +34618,7 @@
         <v>1.52878308229965</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>239</v>
       </c>
@@ -34498,7 +34644,7 @@
         <v>0.245878410585055</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>239</v>
       </c>
@@ -34524,7 +34670,7 @@
         <v>5.1721646693439602</v>
       </c>
     </row>
-    <row r="272" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>239</v>
       </c>
@@ -34550,7 +34696,7 @@
         <v>9.9339868167135095E-2</v>
       </c>
     </row>
-    <row r="273" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>239</v>
       </c>
@@ -34576,7 +34722,7 @@
         <v>3.3995787201406502</v>
       </c>
     </row>
-    <row r="274" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>239</v>
       </c>
@@ -34599,7 +34745,7 @@
         <v>1.0975865950481101</v>
       </c>
     </row>
-    <row r="275" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>239</v>
       </c>
@@ -34622,7 +34768,7 @@
         <v>0.63571915518518796</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>239</v>
       </c>
@@ -34642,7 +34788,7 @@
         <v>-0.27020532089518301</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>239</v>
       </c>
@@ -34662,7 +34808,7 @@
         <v>3.9416833811716501</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>239</v>
       </c>
@@ -34682,7 +34828,7 @@
         <v>-0.22243478035761599</v>
       </c>
     </row>
-    <row r="279" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>254</v>
       </c>
@@ -34713,12 +34859,8 @@
       <c r="L279">
         <v>5.4878314859762201</v>
       </c>
-      <c r="M279">
-        <f t="shared" si="4"/>
-        <v>2.4152650029762199</v>
-      </c>
-    </row>
-    <row r="280" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="280" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>254</v>
       </c>
@@ -34749,12 +34891,8 @@
       <c r="L280">
         <v>3.4490510379286401</v>
       </c>
-      <c r="M280">
-        <f t="shared" si="4"/>
-        <v>0.37648455492863997</v>
-      </c>
-    </row>
-    <row r="281" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="281" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>254</v>
       </c>
@@ -34783,7 +34921,7 @@
         <v>2.6355197882565702</v>
       </c>
     </row>
-    <row r="282" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>254</v>
       </c>
@@ -34812,7 +34950,7 @@
         <v>6.96203428166427E-2</v>
       </c>
     </row>
-    <row r="283" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>254</v>
       </c>
@@ -34841,7 +34979,7 @@
         <v>2.1226682032337001</v>
       </c>
     </row>
-    <row r="284" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>254</v>
       </c>
@@ -34870,7 +35008,7 @@
         <v>1.3284198015190201</v>
       </c>
     </row>
-    <row r="285" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>254</v>
       </c>
@@ -34893,7 +35031,7 @@
         <v>7.4507195586610502</v>
       </c>
     </row>
-    <row r="286" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>254</v>
       </c>
@@ -34916,7 +35054,7 @@
         <v>-2.6065965811994801E-2</v>
       </c>
     </row>
-    <row r="287" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>262</v>
       </c>
@@ -34953,12 +35091,12 @@
       <c r="L287">
         <v>6.5935711804741002E-4</v>
       </c>
-      <c r="M287">
+      <c r="O287">
         <f t="shared" si="4"/>
-        <v>0.99212673811804741</v>
-      </c>
-    </row>
-    <row r="288" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.0573602325821025</v>
+      </c>
+    </row>
+    <row r="288" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>262</v>
       </c>
@@ -34995,12 +35133,12 @@
       <c r="L288">
         <v>5.8849285140168801</v>
       </c>
-      <c r="M288">
+      <c r="O288">
         <f t="shared" si="4"/>
-        <v>7.4416990880168798</v>
-      </c>
-    </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.45">
+        <v>7.4009400812894395</v>
+      </c>
+    </row>
+    <row r="289" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>265</v>
       </c>
@@ -35034,12 +35172,12 @@
       <c r="L289">
         <v>1.8538857140790601</v>
       </c>
-      <c r="M289">
+      <c r="O289">
         <f t="shared" si="4"/>
-        <v>8.2855291920939989E-2</v>
-      </c>
-    </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.23012713877698987</v>
+      </c>
+    </row>
+    <row r="290" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>265</v>
       </c>
@@ -35073,12 +35211,12 @@
       <c r="L290">
         <v>6.3636634872658302</v>
       </c>
-      <c r="M290">
+      <c r="O290">
         <f t="shared" si="4"/>
-        <v>4.4907069892658305</v>
-      </c>
-    </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.45">
+        <v>4.5131421078307898</v>
+      </c>
+    </row>
+    <row r="291" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>265</v>
       </c>
@@ -35100,14 +35238,21 @@
       <c r="G291">
         <v>4.0325043343135798</v>
       </c>
+      <c r="H291">
+        <v>4.3572243571501899</v>
+      </c>
       <c r="I291">
         <v>4.1152961201865699</v>
       </c>
       <c r="J291">
         <v>4.1252569340242102</v>
       </c>
-    </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O291">
+        <f t="shared" si="4"/>
+        <v>1.3320375381501899</v>
+      </c>
+    </row>
+    <row r="292" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>265</v>
       </c>
@@ -35129,14 +35274,21 @@
       <c r="G292">
         <v>5.3079527480975202</v>
       </c>
+      <c r="H292">
+        <v>5.25249875392542</v>
+      </c>
       <c r="I292">
         <v>5.9382437227114604</v>
       </c>
       <c r="J292">
         <v>5.9586850165639502</v>
       </c>
-    </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O292">
+        <f t="shared" si="4"/>
+        <v>1.0283199819254198</v>
+      </c>
+    </row>
+    <row r="293" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>270</v>
       </c>
@@ -35173,12 +35325,12 @@
       <c r="L293">
         <v>-2.6576529658463999</v>
       </c>
-      <c r="M293">
+      <c r="O293">
         <f t="shared" si="4"/>
-        <v>1.5665258061536003</v>
-      </c>
-    </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.45">
+        <v>3.7843257001794841</v>
+      </c>
+    </row>
+    <row r="294" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>270</v>
       </c>
@@ -35215,12 +35367,12 @@
       <c r="L294">
         <v>-3.6654089874752098</v>
       </c>
-      <c r="M294">
+      <c r="O294">
         <f t="shared" si="4"/>
-        <v>1.3779712214752098</v>
-      </c>
-    </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.8335950533525702</v>
+      </c>
+    </row>
+    <row r="295" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>270</v>
       </c>
@@ -35242,6 +35394,9 @@
       <c r="G295">
         <v>-1.0598100086967399</v>
       </c>
+      <c r="H295">
+        <v>-2.6925482187320302</v>
+      </c>
       <c r="I295">
         <v>0.26995821734826603</v>
       </c>
@@ -35251,8 +35406,12 @@
       <c r="K295">
         <v>0.780004412714424</v>
       </c>
-    </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O295">
+        <f t="shared" si="4"/>
+        <v>0.34132594473203026</v>
+      </c>
+    </row>
+    <row r="296" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>270</v>
       </c>
@@ -35274,6 +35433,9 @@
       <c r="G296">
         <v>-2.0314646438574502</v>
       </c>
+      <c r="H296">
+        <v>-1.6095053532035399</v>
+      </c>
       <c r="I296">
         <v>-1.5550434762937499</v>
       </c>
@@ -35283,8 +35445,12 @@
       <c r="K296">
         <v>0.79394604083536202</v>
       </c>
-    </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O296">
+        <f t="shared" si="4"/>
+        <v>0.41051340020353999</v>
+      </c>
+    </row>
+    <row r="297" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>275</v>
       </c>
@@ -35321,12 +35487,12 @@
       <c r="L297">
         <v>-3.1056052173576898</v>
       </c>
-      <c r="M297">
+      <c r="O297">
         <f t="shared" si="4"/>
-        <v>8.0418398357689824E-2</v>
-      </c>
-    </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.71869661332917012</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>275</v>
       </c>
@@ -35363,12 +35529,12 @@
       <c r="L298">
         <v>-1.52991409506284E-2</v>
       </c>
-      <c r="M298">
+      <c r="O298">
         <f t="shared" si="4"/>
-        <v>1.0731466720493716</v>
-      </c>
-    </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.2782728187149601</v>
+      </c>
+    </row>
+    <row r="299" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>275</v>
       </c>
@@ -35390,6 +35556,9 @@
       <c r="G299">
         <v>-4.6010888745604397E-2</v>
       </c>
+      <c r="H299">
+        <v>0.27235917544872701</v>
+      </c>
       <c r="I299">
         <v>0.25891527730618602</v>
       </c>
@@ -35399,8 +35568,12 @@
       <c r="K299">
         <v>0</v>
       </c>
-    </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O299">
+        <f t="shared" si="4"/>
+        <v>1.4245894974487272</v>
+      </c>
+    </row>
+    <row r="300" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>275</v>
       </c>
@@ -35422,6 +35595,9 @@
       <c r="G300">
         <v>1.7498739523209601</v>
       </c>
+      <c r="H300">
+        <v>2.7022852747133501</v>
+      </c>
       <c r="I300">
         <v>2.4748965366533402</v>
       </c>
@@ -35431,8 +35607,12 @@
       <c r="K300">
         <v>1.5113909568141</v>
       </c>
-    </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O300">
+        <f t="shared" si="4"/>
+        <v>1.5032933217133502</v>
+      </c>
+    </row>
+    <row r="301" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>280</v>
       </c>
@@ -35469,12 +35649,12 @@
       <c r="L301">
         <v>-3.62389203777852</v>
       </c>
-      <c r="M301">
+      <c r="O301">
         <f t="shared" si="4"/>
-        <v>1.75093553977852</v>
-      </c>
-    </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.6923005692162298</v>
+      </c>
+    </row>
+    <row r="302" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>280</v>
       </c>
@@ -35511,12 +35691,12 @@
       <c r="L302">
         <v>-1.3453154496376101</v>
       </c>
-      <c r="M302">
+      <c r="O302">
         <f t="shared" si="4"/>
-        <v>1.40909995763761</v>
-      </c>
-    </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.4151591561326899</v>
+      </c>
+    </row>
+    <row r="303" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>280</v>
       </c>
@@ -35538,14 +35718,21 @@
       <c r="G303">
         <v>1.20268617247775</v>
       </c>
+      <c r="H303">
+        <v>0.66969967021285803</v>
+      </c>
       <c r="I303">
         <v>0.77446031469980803</v>
       </c>
       <c r="J303">
         <v>1.30029848222066</v>
       </c>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O303">
+        <f t="shared" si="4"/>
+        <v>0.48253065178714205</v>
+      </c>
+    </row>
+    <row r="304" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>280</v>
       </c>
@@ -35567,14 +35754,21 @@
       <c r="G304">
         <v>1.84789201741414</v>
       </c>
+      <c r="H304">
+        <v>1.51651330546628</v>
+      </c>
       <c r="I304">
         <v>1.59935214936649</v>
       </c>
       <c r="J304">
         <v>2.2463078758869401</v>
       </c>
-    </row>
-    <row r="305" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O304">
+        <f t="shared" si="4"/>
+        <v>0.8347089685337199</v>
+      </c>
+    </row>
+    <row r="305" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>285</v>
       </c>
@@ -35611,12 +35805,12 @@
       <c r="L305">
         <v>0.18191761605094101</v>
       </c>
-      <c r="M305">
+      <c r="O305">
         <f t="shared" si="4"/>
-        <v>2.1186586220509409</v>
-      </c>
-    </row>
-    <row r="306" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.664791375295934</v>
+      </c>
+    </row>
+    <row r="306" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>285</v>
       </c>
@@ -35653,12 +35847,12 @@
       <c r="L306">
         <v>1.6722607745517899</v>
       </c>
-      <c r="M306">
+      <c r="O306">
         <f t="shared" si="4"/>
-        <v>1.7360452825517898</v>
-      </c>
-    </row>
-    <row r="307" spans="1:13" x14ac:dyDescent="0.45">
+        <v>2.0366679439589501</v>
+      </c>
+    </row>
+    <row r="307" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>285</v>
       </c>
@@ -35680,6 +35874,9 @@
       <c r="G307">
         <v>3.8413980533520302</v>
       </c>
+      <c r="H307">
+        <v>3.9728991813169099</v>
+      </c>
       <c r="I307">
         <v>3.4427281903257598</v>
       </c>
@@ -35689,8 +35886,12 @@
       <c r="K307">
         <v>4.3527722595093996</v>
       </c>
-    </row>
-    <row r="308" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O307">
+        <f t="shared" si="4"/>
+        <v>2.88445336831691</v>
+      </c>
+    </row>
+    <row r="308" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>285</v>
       </c>
@@ -35712,6 +35913,9 @@
       <c r="G308">
         <v>5.44660580627282</v>
       </c>
+      <c r="H308">
+        <v>5.4558430672037304</v>
+      </c>
       <c r="I308">
         <v>5.7867155799188303</v>
       </c>
@@ -35721,8 +35925,12 @@
       <c r="K308">
         <v>5.1329443693536598</v>
       </c>
-    </row>
-    <row r="309" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O308">
+        <f t="shared" si="4"/>
+        <v>3.1684053012037303</v>
+      </c>
+    </row>
+    <row r="309" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>290</v>
       </c>
@@ -35750,12 +35958,8 @@
       <c r="L309">
         <v>0.53233379805519598</v>
       </c>
-      <c r="M309">
-        <f t="shared" si="4"/>
-        <v>0.38712098605519596</v>
-      </c>
-    </row>
-    <row r="310" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="310" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>290</v>
       </c>
@@ -35783,12 +35987,8 @@
       <c r="L310">
         <v>-1.86088941329137</v>
       </c>
-      <c r="M310">
-        <f t="shared" si="4"/>
-        <v>1.8206114552913699</v>
-      </c>
-    </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="311" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>290</v>
       </c>
@@ -35811,7 +36011,7 @@
         <v>-2.5626768800848301</v>
       </c>
     </row>
-    <row r="312" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>290</v>
       </c>
@@ -35834,7 +36034,7 @@
         <v>5.17141702636763E-2</v>
       </c>
     </row>
-    <row r="313" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>290</v>
       </c>
@@ -35854,7 +36054,7 @@
         <v>2.9963756513279802E-2</v>
       </c>
     </row>
-    <row r="314" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>290</v>
       </c>
@@ -35874,7 +36074,7 @@
         <v>-0.74032314943819899</v>
       </c>
     </row>
-    <row r="315" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>290</v>
       </c>
@@ -35891,7 +36091,7 @@
         <v>-1.1939254171011199E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>290</v>
       </c>
@@ -35908,7 +36108,7 @@
         <v>6.1870885684129</v>
       </c>
     </row>
-    <row r="317" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>290</v>
       </c>
@@ -35925,7 +36125,7 @@
         <v>2.5979327954657001</v>
       </c>
     </row>
-    <row r="318" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>290</v>
       </c>
@@ -35942,7 +36142,7 @@
         <v>2.5842686288185099</v>
       </c>
     </row>
-    <row r="319" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>300</v>
       </c>
@@ -35979,12 +36179,12 @@
       <c r="L319">
         <v>-1.0122855732502101</v>
       </c>
-      <c r="M319">
+      <c r="O319">
         <f t="shared" si="4"/>
-        <v>0.15005718925021005</v>
-      </c>
-    </row>
-    <row r="320" spans="1:13" x14ac:dyDescent="0.45">
+        <v>0.32308085859868696</v>
+      </c>
+    </row>
+    <row r="320" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>302</v>
       </c>
@@ -36021,12 +36221,12 @@
       <c r="L320">
         <v>-0.75173941463231098</v>
       </c>
-      <c r="M320">
+      <c r="O320">
         <f t="shared" si="4"/>
-        <v>3.084571268632311</v>
-      </c>
-    </row>
-    <row r="321" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.8700794348174572</v>
+      </c>
+    </row>
+    <row r="321" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>302</v>
       </c>
@@ -36063,12 +36263,12 @@
       <c r="L321">
         <v>4.7059553818407496</v>
       </c>
-      <c r="M321">
+      <c r="O321">
         <f t="shared" si="4"/>
-        <v>3.3248330288407493</v>
-      </c>
-    </row>
-    <row r="322" spans="1:13" x14ac:dyDescent="0.45">
+        <v>3.3887766512701401</v>
+      </c>
+    </row>
+    <row r="322" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A322" t="s">
         <v>302</v>
       </c>
@@ -36090,6 +36290,9 @@
       <c r="G322">
         <v>0.108626232400183</v>
       </c>
+      <c r="H322">
+        <v>0.294959002964296</v>
+      </c>
       <c r="I322">
         <v>-1.0068951169549101</v>
       </c>
@@ -36099,8 +36302,12 @@
       <c r="K322">
         <v>0.239636585601783</v>
       </c>
-    </row>
-    <row r="323" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O322">
+        <f t="shared" si="4"/>
+        <v>0.58996307003570403</v>
+      </c>
+    </row>
+    <row r="323" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A323" t="s">
         <v>302</v>
       </c>
@@ -36122,6 +36329,9 @@
       <c r="G323">
         <v>3.0000331202816999</v>
       </c>
+      <c r="H323">
+        <v>2.9544510025566399</v>
+      </c>
       <c r="I323">
         <v>3.38507245826194</v>
       </c>
@@ -36131,8 +36341,12 @@
       <c r="K323">
         <v>1.3358908492303201</v>
       </c>
-    </row>
-    <row r="324" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O323">
+        <f t="shared" ref="O323:O386" si="5">ABS(H323-C323)</f>
+        <v>1.6630525874433602</v>
+      </c>
+    </row>
+    <row r="324" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A324" t="s">
         <v>302</v>
       </c>
@@ -36164,7 +36378,7 @@
         <v>-0.206443015805052</v>
       </c>
     </row>
-    <row r="325" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A325" t="s">
         <v>302</v>
       </c>
@@ -36196,7 +36410,7 @@
         <v>0.109291400866004</v>
       </c>
     </row>
-    <row r="326" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A326" t="s">
         <v>302</v>
       </c>
@@ -36225,7 +36439,7 @@
         <v>-0.70447346550818102</v>
       </c>
     </row>
-    <row r="327" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A327" t="s">
         <v>302</v>
       </c>
@@ -36254,7 +36468,7 @@
         <v>0.43358140221835101</v>
       </c>
     </row>
-    <row r="328" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A328" t="s">
         <v>302</v>
       </c>
@@ -36283,7 +36497,7 @@
         <v>-3.9003284840085102</v>
       </c>
     </row>
-    <row r="329" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A329" t="s">
         <v>302</v>
       </c>
@@ -36312,7 +36526,7 @@
         <v>0.78478758033534102</v>
       </c>
     </row>
-    <row r="330" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A330" t="s">
         <v>311</v>
       </c>
@@ -36349,12 +36563,12 @@
       <c r="L330">
         <v>0.16984080579009</v>
       </c>
-      <c r="M330">
-        <f t="shared" ref="M330:M384" si="5">ABS(L330-C330)</f>
-        <v>0.33315601379008997</v>
-      </c>
-    </row>
-    <row r="331" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O330">
+        <f t="shared" si="5"/>
+        <v>0.17256036488514473</v>
+      </c>
+    </row>
+    <row r="331" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A331" t="s">
         <v>311</v>
       </c>
@@ -36391,12 +36605,12 @@
       <c r="L331">
         <v>-1.00226886877871</v>
       </c>
-      <c r="M331">
+      <c r="O331">
         <f t="shared" si="5"/>
-        <v>1.0960240977787099</v>
-      </c>
-    </row>
-    <row r="332" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.019856434304657</v>
+      </c>
+    </row>
+    <row r="332" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A332" t="s">
         <v>311</v>
       </c>
@@ -36418,6 +36632,9 @@
       <c r="G332">
         <v>0.55431129594339801</v>
       </c>
+      <c r="H332">
+        <v>0.52803081818935405</v>
+      </c>
       <c r="I332">
         <v>0.457399296322273</v>
       </c>
@@ -36427,8 +36644,12 @@
       <c r="K332">
         <v>1.41363281351004</v>
       </c>
-    </row>
-    <row r="333" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O332">
+        <f t="shared" si="5"/>
+        <v>0.761160272189354</v>
+      </c>
+    </row>
+    <row r="333" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A333" t="s">
         <v>311</v>
       </c>
@@ -36450,6 +36671,9 @@
       <c r="G333">
         <v>-5.8445134001294703E-2</v>
       </c>
+      <c r="H333">
+        <v>9.5748779825989894E-2</v>
+      </c>
       <c r="I333">
         <v>-8.70598918053474E-2</v>
       </c>
@@ -36459,8 +36683,12 @@
       <c r="K333">
         <v>-4.8971653186799802E-2</v>
       </c>
-    </row>
-    <row r="334" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O333">
+        <f t="shared" si="5"/>
+        <v>1.9935508259898982E-3</v>
+      </c>
+    </row>
+    <row r="334" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A334" t="s">
         <v>311</v>
       </c>
@@ -36492,7 +36720,7 @@
         <v>-0.57165297157589501</v>
       </c>
     </row>
-    <row r="335" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A335" t="s">
         <v>315</v>
       </c>
@@ -36529,12 +36757,12 @@
       <c r="L335">
         <v>-2.54381972308801</v>
       </c>
-      <c r="M335">
+      <c r="O335">
         <f t="shared" si="5"/>
-        <v>3.2206014990880099</v>
-      </c>
-    </row>
-    <row r="336" spans="1:13" x14ac:dyDescent="0.45">
+        <v>3.3968765382460298</v>
+      </c>
+    </row>
+    <row r="336" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A336" t="s">
         <v>315</v>
       </c>
@@ -36571,12 +36799,12 @@
       <c r="L336">
         <v>-4.3383873620692599</v>
       </c>
-      <c r="M336">
+      <c r="O336">
         <f t="shared" si="5"/>
-        <v>5.2475949560692596</v>
-      </c>
-    </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.45">
+        <v>5.2253661517907597</v>
+      </c>
+    </row>
+    <row r="337" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A337" t="s">
         <v>315</v>
       </c>
@@ -36598,6 +36826,9 @@
       <c r="G337">
         <v>0.86036420194577601</v>
       </c>
+      <c r="H337">
+        <v>-2.0502628354242901E-2</v>
+      </c>
       <c r="I337">
         <v>-0.29802814334134298</v>
       </c>
@@ -36607,8 +36838,12 @@
       <c r="K337">
         <v>0</v>
       </c>
-    </row>
-    <row r="338" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O337">
+        <f t="shared" si="5"/>
+        <v>0.1579664913542429</v>
+      </c>
+    </row>
+    <row r="338" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A338" t="s">
         <v>315</v>
       </c>
@@ -36630,6 +36865,9 @@
       <c r="G338">
         <v>-0.22741395429698</v>
       </c>
+      <c r="H338">
+        <v>-2.6766325079352098E-2</v>
+      </c>
       <c r="I338">
         <v>5.0262789430507798E-2</v>
       </c>
@@ -36639,8 +36877,12 @@
       <c r="K338">
         <v>-7.2145438984352897E-2</v>
       </c>
-    </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="O338">
+        <f t="shared" si="5"/>
+        <v>1.4825822520793521</v>
+      </c>
+    </row>
+    <row r="339" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A339" t="s">
         <v>315</v>
       </c>
@@ -36672,7 +36914,7 @@
         <v>5.8965785814398197</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A340" t="s">
         <v>315</v>
       </c>
@@ -36704,7 +36946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A341" t="s">
         <v>315</v>
       </c>
@@ -36736,7 +36978,7 @@
         <v>-0.27010443897402098</v>
       </c>
     </row>
-    <row r="342" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A342" t="s">
         <v>315</v>
       </c>
@@ -36768,7 +37010,7 @@
         <v>1.09111955423941E-2</v>
       </c>
     </row>
-    <row r="343" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A343" t="s">
         <v>315</v>
       </c>
@@ -36800,7 +37042,7 @@
         <v>0.74857525119618895</v>
       </c>
     </row>
-    <row r="344" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A344" t="s">
         <v>315</v>
       </c>
@@ -36832,7 +37074,7 @@
         <v>0.57564041386876796</v>
       </c>
     </row>
-    <row r="345" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A345" t="s">
         <v>315</v>
       </c>
@@ -36861,7 +37103,7 @@
         <v>0.13472757370600399</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A346" t="s">
         <v>315</v>
       </c>
@@ -36890,7 +37132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A347" t="s">
         <v>328</v>
       </c>
@@ -36918,12 +37160,8 @@
       <c r="L347">
         <v>1.2288841093432401</v>
       </c>
-      <c r="M347">
-        <f t="shared" si="5"/>
-        <v>0.90479323234324016</v>
-      </c>
-    </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="348" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A348" t="s">
         <v>328</v>
       </c>
@@ -36951,12 +37189,8 @@
       <c r="L348">
         <v>0.12576591072979601</v>
       </c>
-      <c r="M348">
-        <f t="shared" si="5"/>
-        <v>1.029078403729796</v>
-      </c>
-    </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="349" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A349" t="s">
         <v>328</v>
       </c>
@@ -36979,7 +37213,7 @@
         <v>0.23704698879928399</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A350" t="s">
         <v>328</v>
       </c>
@@ -37002,7 +37236,7 @@
         <v>-0.71622163424817697</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A351" t="s">
         <v>328</v>
       </c>
@@ -37016,7 +37250,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="352" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A352" t="s">
         <v>328</v>
       </c>
@@ -37030,7 +37264,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="353" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A353" t="s">
         <v>328</v>
       </c>
@@ -37044,7 +37278,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A354" t="s">
         <v>328</v>
       </c>
@@ -37058,7 +37292,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A355" t="s">
         <v>335</v>
       </c>
@@ -37086,12 +37320,8 @@
       <c r="L355">
         <v>2.0688650910880302</v>
       </c>
-      <c r="M355">
-        <f t="shared" si="5"/>
-        <v>2.1092752030880302</v>
-      </c>
-    </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="356" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A356" t="s">
         <v>335</v>
       </c>
@@ -37119,12 +37349,8 @@
       <c r="L356">
         <v>1.43595770886049</v>
       </c>
-      <c r="M356">
-        <f t="shared" si="5"/>
-        <v>7.3268364139509989E-2</v>
-      </c>
-    </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="357" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A357" t="s">
         <v>335</v>
       </c>
@@ -37150,7 +37376,7 @@
         <v>3.75411010699945</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A358" t="s">
         <v>335</v>
       </c>
@@ -37176,7 +37402,7 @@
         <v>2.2815988238517</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A359" t="s">
         <v>335</v>
       </c>
@@ -37196,7 +37422,7 @@
         <v>1.61283674738424</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A360" t="s">
         <v>335</v>
       </c>
@@ -37216,7 +37442,7 @@
         <v>5.3888783741228501</v>
       </c>
     </row>
-    <row r="361" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A361" t="s">
         <v>335</v>
       </c>
@@ -37233,7 +37459,7 @@
         <v>0.67960432059780895</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A362" t="s">
         <v>335</v>
       </c>
@@ -37250,7 +37476,7 @@
         <v>2.5433549646868401</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A363" t="s">
         <v>335</v>
       </c>
@@ -37264,7 +37490,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A364" t="s">
         <v>335</v>
       </c>
@@ -37278,7 +37504,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="365" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A365" t="s">
         <v>335</v>
       </c>
@@ -37292,7 +37518,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A366" t="s">
         <v>335</v>
       </c>
@@ -37306,7 +37532,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="367" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A367" t="s">
         <v>335</v>
       </c>
@@ -37320,7 +37546,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A368" t="s">
         <v>335</v>
       </c>
@@ -37334,7 +37560,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="369" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A369" t="s">
         <v>335</v>
       </c>
@@ -37348,7 +37574,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="370" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A370" t="s">
         <v>335</v>
       </c>
@@ -37362,7 +37588,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="371" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A371" t="s">
         <v>335</v>
       </c>
@@ -37376,7 +37602,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="372" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A372" t="s">
         <v>335</v>
       </c>
@@ -37390,7 +37616,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="373" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A373" t="s">
         <v>335</v>
       </c>
@@ -37404,7 +37630,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="374" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A374" t="s">
         <v>335</v>
       </c>
@@ -37418,7 +37644,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="375" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A375" t="s">
         <v>335</v>
       </c>
@@ -37432,7 +37658,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="376" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A376" t="s">
         <v>335</v>
       </c>
@@ -37446,7 +37672,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="377" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A377" t="s">
         <v>335</v>
       </c>
@@ -37460,7 +37686,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="378" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A378" t="s">
         <v>335</v>
       </c>
@@ -37474,7 +37700,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="379" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A379" t="s">
         <v>335</v>
       </c>
@@ -37488,7 +37714,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="380" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A380" t="s">
         <v>335</v>
       </c>
@@ -37502,7 +37728,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="381" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A381" t="s">
         <v>335</v>
       </c>
@@ -37516,7 +37742,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="382" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A382" t="s">
         <v>335</v>
       </c>
@@ -37530,7 +37756,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="383" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A383" t="s">
         <v>363</v>
       </c>
@@ -37567,12 +37793,12 @@
       <c r="L383">
         <v>-0.51075631300503799</v>
       </c>
-      <c r="M383">
+      <c r="O383">
         <f t="shared" si="5"/>
-        <v>1.710785894005038</v>
-      </c>
-    </row>
-    <row r="384" spans="1:13" x14ac:dyDescent="0.45">
+        <v>1.3194474615608949</v>
+      </c>
+    </row>
+    <row r="384" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A384" t="s">
         <v>363</v>
       </c>
@@ -37609,12 +37835,12 @@
       <c r="L384">
         <v>1.0678115303797799</v>
       </c>
-      <c r="M384">
+      <c r="O384">
         <f t="shared" si="5"/>
-        <v>0.57616667337977989</v>
-      </c>
-    </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.45">
+        <v>0.485814565039762</v>
+      </c>
+    </row>
+    <row r="385" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A385" t="s">
         <v>363</v>
       </c>
@@ -37637,7 +37863,7 @@
         <v>-0.14272601229326901</v>
       </c>
       <c r="H385">
-        <v>-0.39729046514652899</v>
+        <v>-0.227861375864335</v>
       </c>
       <c r="I385">
         <v>-0.177873557325642</v>
@@ -37648,8 +37874,12 @@
       <c r="K385">
         <v>-0.29189128881744097</v>
       </c>
-    </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O385">
+        <f t="shared" si="5"/>
+        <v>0.28962267986433499</v>
+      </c>
+    </row>
+    <row r="386" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A386" t="s">
         <v>363</v>
       </c>
@@ -37672,7 +37902,7 @@
         <v>1.9784651384171801</v>
       </c>
       <c r="H386">
-        <v>1.49201197353681</v>
+        <v>1.7420039192239001</v>
       </c>
       <c r="I386">
         <v>1.43578333499528</v>
@@ -37683,8 +37913,12 @@
       <c r="K386">
         <v>1.83224921367664</v>
       </c>
-    </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O386">
+        <f t="shared" si="5"/>
+        <v>2.1424776097760998</v>
+      </c>
+    </row>
+    <row r="387" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A387" t="s">
         <v>363</v>
       </c>
@@ -37706,6 +37940,9 @@
       <c r="G387">
         <v>0.98438872009543199</v>
       </c>
+      <c r="H387">
+        <v>0.25220496826012301</v>
+      </c>
       <c r="I387">
         <v>1.0178886253364601</v>
       </c>
@@ -37715,8 +37952,12 @@
       <c r="K387">
         <v>0.15254654966111</v>
       </c>
-    </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O387">
+        <f t="shared" ref="O387:O388" si="6">ABS(H387-C387)</f>
+        <v>0.69643619473987695</v>
+      </c>
+    </row>
+    <row r="388" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A388" t="s">
         <v>363</v>
       </c>
@@ -37738,6 +37979,9 @@
       <c r="G388">
         <v>3.4072713788355999</v>
       </c>
+      <c r="H388">
+        <v>2.6757311355870299</v>
+      </c>
       <c r="I388">
         <v>2.9881477710629198</v>
       </c>
@@ -37747,8 +37991,12 @@
       <c r="K388">
         <v>2.3570519136067101</v>
       </c>
-    </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="O388">
+        <f t="shared" si="6"/>
+        <v>1.0471435654129699</v>
+      </c>
+    </row>
+    <row r="389" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A389" t="s">
         <v>363</v>
       </c>
@@ -37780,7 +38028,7 @@
         <v>-0.19602802374943101</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A390" t="s">
         <v>363</v>
       </c>
@@ -37812,7 +38060,7 @@
         <v>3.5126893413815599</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A391" t="s">
         <v>363</v>
       </c>
@@ -37844,7 +38092,7 @@
         <v>1.73287998551345</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A392" t="s">
         <v>363</v>
       </c>
@@ -37876,7 +38124,7 @@
         <v>7.2236469669087394E-2</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A393" t="s">
         <v>363</v>
       </c>
@@ -37908,7 +38156,7 @@
         <v>3.2292070204419798</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A394" t="s">
         <v>363</v>
       </c>
@@ -37940,7 +38188,7 @@
         <v>1.95757332899602</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A395" t="s">
         <v>363</v>
       </c>
@@ -37972,7 +38220,7 @@
         <v>1.8345275574023101</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A396" t="s">
         <v>363</v>
       </c>
@@ -38004,7 +38252,7 @@
         <v>2.8689001213774601</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A397" t="s">
         <v>363</v>
       </c>
@@ -38036,7 +38284,7 @@
         <v>-0.176770279368338</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A398" t="s">
         <v>363</v>
       </c>
@@ -38068,7 +38316,7 @@
         <v>4.7679702276434002</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A399" t="s">
         <v>363</v>
       </c>
@@ -38100,7 +38348,7 @@
         <v>3.42585089767462</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A400" t="s">
         <v>363</v>
       </c>
@@ -38518,7 +38766,7 @@
         <v>-2.46875820324703E-2</v>
       </c>
     </row>
-    <row r="417" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A417" t="s">
         <v>363</v>
       </c>
@@ -38538,7 +38786,7 @@
         <v>-3.5690589221712699E-2</v>
       </c>
     </row>
-    <row r="418" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A418" t="s">
         <v>363</v>
       </c>
@@ -38558,7 +38806,7 @@
         <v>-0.71009588311449001</v>
       </c>
     </row>
-    <row r="419" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A419" t="s">
         <v>363</v>
       </c>
@@ -38578,7 +38826,7 @@
         <v>1.6218985479690601E-2</v>
       </c>
     </row>
-    <row r="420" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A420" t="s">
         <v>378</v>
       </c>
@@ -38603,12 +38851,8 @@
       <c r="L420">
         <v>-0.903279956219594</v>
       </c>
-      <c r="M420">
-        <f t="shared" ref="M420:M430" si="6">ABS(L420-C420)</f>
-        <v>0.77949808921959396</v>
-      </c>
-    </row>
-    <row r="421" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="421" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A421" t="s">
         <v>378</v>
       </c>
@@ -38633,12 +38877,8 @@
       <c r="L421">
         <v>1.1863670678679601</v>
       </c>
-      <c r="M421">
-        <f t="shared" si="6"/>
-        <v>1.1789543838679601</v>
-      </c>
-    </row>
-    <row r="422" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="422" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A422" t="s">
         <v>378</v>
       </c>
@@ -38658,7 +38898,7 @@
         <v>-0.105111008432095</v>
       </c>
     </row>
-    <row r="423" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A423" t="s">
         <v>378</v>
       </c>
@@ -38678,7 +38918,7 @@
         <v>-0.11968725716909</v>
       </c>
     </row>
-    <row r="424" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A424" t="s">
         <v>378</v>
       </c>
@@ -38695,7 +38935,7 @@
         <v>-1.4788898261352299E-2</v>
       </c>
     </row>
-    <row r="425" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A425" t="s">
         <v>378</v>
       </c>
@@ -38712,7 +38952,7 @@
         <v>0.66125751384265896</v>
       </c>
     </row>
-    <row r="426" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A426" t="s">
         <v>378</v>
       </c>
@@ -38726,7 +38966,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="427" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A427" t="s">
         <v>378</v>
       </c>
@@ -38740,7 +38980,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="428" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A428" t="s">
         <v>378</v>
       </c>
@@ -38754,7 +38994,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="429" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A429" t="s">
         <v>389</v>
       </c>
@@ -38782,12 +39022,8 @@
       <c r="L429">
         <v>-0.67631603518029804</v>
       </c>
-      <c r="M429">
-        <f t="shared" si="6"/>
-        <v>8.8587255180298086E-2</v>
-      </c>
-    </row>
-    <row r="430" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="430" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A430" t="s">
         <v>389</v>
       </c>
@@ -38815,12 +39051,8 @@
       <c r="L430">
         <v>-0.69734080456487302</v>
       </c>
-      <c r="M430">
-        <f t="shared" si="6"/>
-        <v>1.5031801635648732</v>
-      </c>
-    </row>
-    <row r="431" spans="1:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="431" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A431" t="s">
         <v>389</v>
       </c>
@@ -38840,7 +39072,7 @@
         <v>0.13319677306108099</v>
       </c>
     </row>
-    <row r="432" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A432" t="s">
         <v>389</v>
       </c>
@@ -39007,7 +39239,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39053,7 +39285,7 @@
       </c>
       <c r="B5">
         <f>PEARSON(Sheet1!C:C, Sheet1!H:H)</f>
-        <v>0.51907340801591118</v>
+        <v>0.59270643099884457</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -39092,8 +39324,8 @@
         <v>0.55726755506560344</v>
       </c>
       <c r="C9">
-        <f>AVERAGE(Sheet1!M:M)</f>
-        <v>1.5520417548812238</v>
+        <f>AVERAGE(Sheet1!O:O)</f>
+        <v>1.4695697223382391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>